<commit_message>
Planning results functions corrected. New parameter added to NetworkParameters. CS1 updated.
</commit_message>
<xml_diff>
--- a/data/CS1/market data/cs1_market_data_2020.xlsx
+++ b/data/CS1/market data/cs1_market_data_2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\shared-resources-planning-v3\data\CS1\market data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B6F39B-6A9E-40EA-A847-AEAA32C491D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118BF958-4FA1-48E2-BA4E-23CA98170941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1950" windowWidth="29040" windowHeight="17640" xr2:uid="{D5815E3E-A825-47B7-91B5-1362E9B2D293}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5815E3E-A825-47B7-91B5-1362E9B2D293}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="5" r:id="rId1"/>

</xml_diff>